<commit_message>
Tests green, refactored tests, archived old
</commit_message>
<xml_diff>
--- a/data/datafile.xlsx
+++ b/data/datafile.xlsx
@@ -1,12 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA55535-7F69-5240-95DB-DF0B0667304A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="home" state="visible" r:id="rId4"/>
+    <sheet name="home" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -64,17 +80,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,14 +113,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="double"/>
+      <left style="double">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -126,7 +149,17 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FF99D07A"/>
+          <bgColor rgb="FFD4EDD2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -141,12 +174,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFC00000"/>
+          <bgColor rgb="FF99D07A"/>
         </patternFill>
       </fill>
     </dxf>
@@ -158,9 +188,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FF99D07A"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -175,19 +208,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD4EDD2"/>
+          <bgColor rgb="FF99D07A"/>
         </patternFill>
       </fill>
     </dxf>
@@ -525,9 +548,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P17"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -545,7 +573,7 @@
     <col min="16" max="16" width="15" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,9 +623,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>0.139</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="B2">
         <v>375</v>
@@ -616,15 +644,19 @@
       </c>
       <c r="G2" s="3">
         <f t="shared" ref="G2:G17" si="0">F2/D2</f>
+        <v>4.4888888888888889</v>
       </c>
       <c r="H2" s="3">
         <f t="shared" ref="H2:H17" si="1">G2/MIN(2,C2)</f>
-      </c>
-      <c r="I2">
+        <v>2.2444444444444445</v>
+      </c>
+      <c r="I2" t="str">
         <f t="shared" ref="I2:I17" si="2">_xlfn.IFS(    H2&lt;0.9, "POOR (--)",     H2&lt;1, "(-)",     H2=1, "GOOD!",     H2&gt;1.2, "BIG (++)",     H2&gt;1, "(+)"  )</f>
+        <v>BIG (++)</v>
       </c>
       <c r="J2" s="1">
         <f t="shared" ref="J2:J17" si="3">(H2-1)*A2</f>
+        <v>0.17297777777777779</v>
       </c>
       <c r="K2" s="4">
         <v>630</v>
@@ -634,20 +666,24 @@
       </c>
       <c r="M2" s="3">
         <f t="shared" ref="M2:M17" si="4">L2/D2</f>
+        <v>2.2476190476190476</v>
       </c>
       <c r="N2" s="3">
         <f t="shared" ref="N2:N17" si="5">M2/MIN(2,C2)</f>
-      </c>
-      <c r="O2">
+        <v>1.1238095238095238</v>
+      </c>
+      <c r="O2" t="str">
         <f t="shared" ref="O2:O17" si="6">_xlfn.IFS(    N2&lt;0.9, "POOR (--)",     N2&lt;1, "(-)",     N2=1, "GOOD!",     N2&gt;1.2, "BIG (++)",     N2&gt;1, "(+)"  )</f>
+        <v>(+)</v>
       </c>
       <c r="P2" s="1">
         <f t="shared" ref="P2:P17" si="7">(N2-1)*A2</f>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1.720952380952381E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>0.134</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="B3">
         <v>414</v>
@@ -666,15 +702,19 @@
       </c>
       <c r="G3" s="3">
         <f t="shared" si="0"/>
+        <v>3.9943502824858759</v>
       </c>
       <c r="H3" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="I3">
+        <v>1.9971751412429379</v>
+      </c>
+      <c r="I3" t="str">
         <f t="shared" si="2"/>
+        <v>BIG (++)</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" si="3"/>
+        <v>0.13362146892655369</v>
       </c>
       <c r="K3" s="4">
         <v>708</v>
@@ -684,20 +724,24 @@
       </c>
       <c r="M3" s="3">
         <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="N3" s="3">
         <f t="shared" si="5"/>
-      </c>
-      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="O3" t="str">
         <f t="shared" si="6"/>
+        <v>GOOD!</v>
       </c>
       <c r="P3" s="1">
         <f t="shared" si="7"/>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>0.095</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="B4">
         <v>390</v>
@@ -716,15 +760,19 @@
       </c>
       <c r="G4" s="3">
         <f t="shared" si="0"/>
+        <v>4.2848484848484851</v>
       </c>
       <c r="H4" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="I4">
+        <v>2.1424242424242426</v>
+      </c>
+      <c r="I4" t="str">
         <f t="shared" si="2"/>
+        <v>BIG (++)</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
+        <v>0.10853030303030305</v>
       </c>
       <c r="K4" s="4">
         <v>660</v>
@@ -734,20 +782,24 @@
       </c>
       <c r="M4" s="3">
         <f t="shared" si="4"/>
+        <v>2.1454545454545455</v>
       </c>
       <c r="N4" s="3">
         <f t="shared" si="5"/>
-      </c>
-      <c r="O4">
+        <v>1.0727272727272728</v>
+      </c>
+      <c r="O4" t="str">
         <f t="shared" si="6"/>
+        <v>(+)</v>
       </c>
       <c r="P4" s="1">
         <f t="shared" si="7"/>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>6.9090909090909116E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>0.086</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="B5">
         <v>375</v>
@@ -766,15 +818,19 @@
       </c>
       <c r="G5" s="3">
         <f t="shared" si="0"/>
+        <v>4.4888888888888889</v>
       </c>
       <c r="H5" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="I5">
+        <v>2.2444444444444445</v>
+      </c>
+      <c r="I5" t="str">
         <f t="shared" si="2"/>
+        <v>BIG (++)</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
+        <v>0.10702222222222221</v>
       </c>
       <c r="K5" s="4">
         <v>630</v>
@@ -784,20 +840,24 @@
       </c>
       <c r="M5" s="3">
         <f t="shared" si="4"/>
+        <v>2.2476190476190476</v>
       </c>
       <c r="N5" s="3">
         <f t="shared" si="5"/>
-      </c>
-      <c r="O5">
+        <v>1.1238095238095238</v>
+      </c>
+      <c r="O5" t="str">
         <f t="shared" si="6"/>
+        <v>(+)</v>
       </c>
       <c r="P5" s="1">
         <f t="shared" si="7"/>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1.0647619047619046E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>0.083</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="B6">
         <v>414</v>
@@ -816,15 +876,19 @@
       </c>
       <c r="G6" s="3">
         <f t="shared" si="0"/>
+        <v>3.9943502824858759</v>
       </c>
       <c r="H6" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="I6">
+        <v>1.9971751412429379</v>
+      </c>
+      <c r="I6" t="str">
         <f t="shared" si="2"/>
+        <v>BIG (++)</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
+        <v>8.2765536723163849E-2</v>
       </c>
       <c r="K6" s="4">
         <v>708</v>
@@ -834,20 +898,24 @@
       </c>
       <c r="M6" s="3">
         <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="N6" s="3">
         <f t="shared" si="5"/>
-      </c>
-      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="O6" t="str">
         <f t="shared" si="6"/>
+        <v>GOOD!</v>
       </c>
       <c r="P6" s="1">
         <f t="shared" si="7"/>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>0.061</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="B7">
         <v>360</v>
@@ -866,15 +934,19 @@
       </c>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
+        <v>4.7133333333333329</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="I7">
+        <v>2.3566666666666665</v>
+      </c>
+      <c r="I7" t="str">
         <f t="shared" si="2"/>
+        <v>BIG (++)</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
+        <v>8.2756666666666659E-2</v>
       </c>
       <c r="K7" s="4">
         <v>600</v>
@@ -884,20 +956,24 @@
       </c>
       <c r="M7" s="3">
         <f t="shared" si="4"/>
+        <v>2.36</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="5"/>
-      </c>
-      <c r="O7">
+        <v>1.18</v>
+      </c>
+      <c r="O7" t="str">
         <f t="shared" si="6"/>
+        <v>(+)</v>
       </c>
       <c r="P7" s="1">
         <f t="shared" si="7"/>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1.0979999999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>0.052000000000000005</v>
+        <v>5.2000000000000005E-2</v>
       </c>
       <c r="B8">
         <v>428</v>
@@ -916,15 +992,19 @@
       </c>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
+        <v>3.8423913043478262</v>
       </c>
       <c r="H8" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="I8">
+        <v>1.9211956521739131</v>
+      </c>
+      <c r="I8" t="str">
         <f t="shared" si="2"/>
+        <v>BIG (++)</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
+        <v>4.7902173913043487E-2</v>
       </c>
       <c r="K8" s="4">
         <v>736</v>
@@ -934,20 +1014,24 @@
       </c>
       <c r="M8" s="3">
         <f t="shared" si="4"/>
+        <v>1.923913043478261</v>
       </c>
       <c r="N8" s="3">
         <f t="shared" si="5"/>
-      </c>
-      <c r="O8">
+        <v>0.96195652173913049</v>
+      </c>
+      <c r="O8" t="str">
         <f t="shared" si="6"/>
+        <v>(-)</v>
       </c>
       <c r="P8" s="1">
         <f t="shared" si="7"/>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <v>-1.9782608695652149E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>0.040999999999999995</v>
+        <v>4.0999999999999995E-2</v>
       </c>
       <c r="B9">
         <v>1920</v>
@@ -966,38 +1050,46 @@
       </c>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
+        <v>2.5249999999999999</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="I9">
+        <v>2.5249999999999999</v>
+      </c>
+      <c r="I9" t="str">
         <f t="shared" si="2"/>
+        <v>BIG (++)</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
+        <v>6.2524999999999983E-2</v>
       </c>
       <c r="K9" s="4">
         <v>560</v>
       </c>
       <c r="L9" s="5">
-        <v>708</v>
+        <v>560</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="5"/>
-      </c>
-      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="O9" t="str">
         <f t="shared" si="6"/>
+        <v>GOOD!</v>
       </c>
       <c r="P9" s="1">
         <f t="shared" si="7"/>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>0.037000000000000005</v>
+        <v>3.7000000000000005E-2</v>
       </c>
       <c r="B10">
         <v>412</v>
@@ -1016,15 +1108,19 @@
       </c>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
+        <v>4.0170454545454541</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="I10">
+        <v>2.0085227272727271</v>
+      </c>
+      <c r="I10" t="str">
         <f t="shared" si="2"/>
+        <v>BIG (++)</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
+        <v>3.7315340909090909E-2</v>
       </c>
       <c r="K10" s="4">
         <v>704</v>
@@ -1034,20 +1130,24 @@
       </c>
       <c r="M10" s="3">
         <f t="shared" si="4"/>
+        <v>2.0113636363636362</v>
       </c>
       <c r="N10" s="3">
         <f t="shared" si="5"/>
-      </c>
-      <c r="O10">
+        <v>1.0056818181818181</v>
+      </c>
+      <c r="O10" t="str">
         <f t="shared" si="6"/>
+        <v>(+)</v>
       </c>
       <c r="P10" s="1">
         <f t="shared" si="7"/>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2.1022727272727051E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>0.023</v>
+        <v>2.3E-2</v>
       </c>
       <c r="B11">
         <v>1440</v>
@@ -1066,38 +1166,46 @@
       </c>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
+        <v>2.6282527881040894</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="I11">
+        <v>1.3141263940520447</v>
+      </c>
+      <c r="I11" t="str">
         <f t="shared" si="2"/>
+        <v>BIG (++)</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
+        <v>7.2249070631970275E-3</v>
       </c>
       <c r="K11" s="4">
         <v>1076</v>
       </c>
       <c r="L11" s="5">
-        <v>708</v>
+        <v>1076</v>
       </c>
       <c r="M11" s="3">
         <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="N11" s="3">
         <f t="shared" si="5"/>
-      </c>
-      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="O11" t="str">
         <f t="shared" si="6"/>
+        <v>GOOD!</v>
       </c>
       <c r="P11" s="1">
         <f t="shared" si="7"/>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>0.018000000000000002</v>
+        <v>1.8000000000000002E-2</v>
       </c>
       <c r="B12">
         <v>1366</v>
@@ -1116,38 +1224,46 @@
       </c>
       <c r="G12" s="3">
         <f t="shared" si="0"/>
+        <v>2.8055555555555554</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="I12">
+        <v>2.8055555555555554</v>
+      </c>
+      <c r="I12" t="str">
         <f t="shared" si="2"/>
+        <v>BIG (++)</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
+        <v>3.2500000000000001E-2</v>
       </c>
       <c r="K12" s="4">
         <v>504</v>
       </c>
       <c r="L12" s="5">
-        <v>708</v>
+        <v>560</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="4"/>
+        <v>1.1111111111111112</v>
       </c>
       <c r="N12" s="3">
         <f t="shared" si="5"/>
-      </c>
-      <c r="O12">
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="O12" t="str">
         <f t="shared" si="6"/>
+        <v>(+)</v>
       </c>
       <c r="P12" s="1">
         <f t="shared" si="7"/>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2.0000000000000009E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>0.016</v>
+        <v>1.6E-2</v>
       </c>
       <c r="B13">
         <v>360</v>
@@ -1166,15 +1282,19 @@
       </c>
       <c r="G13" s="3">
         <f t="shared" si="0"/>
+        <v>4.7133333333333329</v>
       </c>
       <c r="H13" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="I13">
+        <v>2.3566666666666665</v>
+      </c>
+      <c r="I13" t="str">
         <f t="shared" si="2"/>
+        <v>BIG (++)</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="3"/>
+        <v>2.1706666666666662E-2</v>
       </c>
       <c r="K13" s="4">
         <v>600</v>
@@ -1184,20 +1304,24 @@
       </c>
       <c r="M13" s="3">
         <f t="shared" si="4"/>
+        <v>2.36</v>
       </c>
       <c r="N13" s="3">
         <f t="shared" si="5"/>
-      </c>
-      <c r="O13">
+        <v>1.18</v>
+      </c>
+      <c r="O13" t="str">
         <f t="shared" si="6"/>
+        <v>(+)</v>
       </c>
       <c r="P13" s="1">
         <f t="shared" si="7"/>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2.8799999999999989E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>0.015</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="B14">
         <v>768</v>
@@ -1216,38 +1340,46 @@
       </c>
       <c r="G14" s="3">
         <f t="shared" si="0"/>
+        <v>6.1746724890829698</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="I14">
+        <v>3.0873362445414849</v>
+      </c>
+      <c r="I14" t="str">
         <f t="shared" si="2"/>
+        <v>BIG (++)</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="3"/>
+        <v>3.1310043668122275E-2</v>
       </c>
       <c r="K14" s="4">
         <v>458</v>
       </c>
       <c r="L14" s="5">
-        <v>708</v>
+        <v>560</v>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="4"/>
+        <v>2.445414847161572</v>
       </c>
       <c r="N14" s="3">
         <f t="shared" si="5"/>
-      </c>
-      <c r="O14">
+        <v>1.222707423580786</v>
+      </c>
+      <c r="O14" t="str">
         <f t="shared" si="6"/>
+        <v>BIG (++)</v>
       </c>
       <c r="P14" s="1">
         <f t="shared" si="7"/>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>3.3406113537117897E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>0.013999999999999999</v>
+        <v>1.3999999999999999E-2</v>
       </c>
       <c r="B15">
         <v>393</v>
@@ -1266,15 +1398,19 @@
       </c>
       <c r="G15" s="3">
         <f t="shared" si="0"/>
+        <v>4.2462462462462458</v>
       </c>
       <c r="H15" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="I15">
+        <v>2.1231231231231229</v>
+      </c>
+      <c r="I15" t="str">
         <f t="shared" si="2"/>
+        <v>BIG (++)</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="3"/>
+        <v>1.5723723723723718E-2</v>
       </c>
       <c r="K15" s="4">
         <v>666</v>
@@ -1284,20 +1420,24 @@
       </c>
       <c r="M15" s="3">
         <f t="shared" si="4"/>
+        <v>2.1261261261261262</v>
       </c>
       <c r="N15" s="3">
         <f t="shared" si="5"/>
-      </c>
-      <c r="O15">
+        <v>1.0630630630630631</v>
+      </c>
+      <c r="O15" t="str">
         <f t="shared" si="6"/>
+        <v>(+)</v>
       </c>
       <c r="P15" s="1">
         <f t="shared" si="7"/>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>8.828828828828831E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>0.011000000000000001</v>
+        <v>1.1000000000000001E-2</v>
       </c>
       <c r="B16">
         <v>1536</v>
@@ -1316,15 +1456,19 @@
       </c>
       <c r="G16" s="3">
         <f t="shared" si="0"/>
+        <v>2.5249999999999999</v>
       </c>
       <c r="H16" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="I16">
+        <v>2.02</v>
+      </c>
+      <c r="I16" t="str">
         <f t="shared" si="2"/>
+        <v>BIG (++)</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="3"/>
+        <v>1.1220000000000001E-2</v>
       </c>
       <c r="K16" s="4">
         <v>700</v>
@@ -1334,20 +1478,24 @@
       </c>
       <c r="M16" s="3">
         <f t="shared" si="4"/>
+        <v>1.2642857142857142</v>
       </c>
       <c r="N16" s="3">
         <f t="shared" si="5"/>
-      </c>
-      <c r="O16">
+        <v>1.0114285714285713</v>
+      </c>
+      <c r="O16" t="str">
         <f t="shared" si="6"/>
+        <v>(+)</v>
       </c>
       <c r="P16" s="1">
         <f t="shared" si="7"/>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1.257142857142848E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>0.008</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="B17">
         <v>320</v>
@@ -1366,65 +1514,73 @@
       </c>
       <c r="G17" s="3">
         <f t="shared" si="0"/>
+        <v>5.4384615384615387</v>
       </c>
       <c r="H17" s="3">
         <f t="shared" si="1"/>
-      </c>
-      <c r="I17">
+        <v>2.7192307692307693</v>
+      </c>
+      <c r="I17" t="str">
         <f t="shared" si="2"/>
+        <v>BIG (++)</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="3"/>
+        <v>1.3753846153846155E-2</v>
       </c>
       <c r="K17" s="4">
         <v>520</v>
       </c>
       <c r="L17" s="5">
-        <v>708</v>
+        <v>560</v>
       </c>
       <c r="M17" s="3">
         <f t="shared" si="4"/>
+        <v>2.1538461538461537</v>
       </c>
       <c r="N17" s="3">
         <f t="shared" si="5"/>
-      </c>
-      <c r="O17">
+        <v>1.0769230769230769</v>
+      </c>
+      <c r="O17" t="str">
         <f t="shared" si="6"/>
+        <v>(+)</v>
       </c>
       <c r="P17" s="1">
         <f t="shared" si="7"/>
+        <v>6.1538461538461497E-4</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L17">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>O2="GOOD!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>O2="POOR (--)"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>O2="BIG (++)"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>OR(O2="(+)",O2="(-)")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F17">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>I2="GOOD!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>I2="POOR (--)"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>I2="BIG (++)"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>OR(I2="(+)",I2="(-)")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tests green for web.dev
</commit_message>
<xml_diff>
--- a/data/datafile.xlsx
+++ b/data/datafile.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DC31B3-C9F4-3745-85A1-EA802EAC39C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FA3F03-FD8F-D546-98A4-3E235DAAA308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="webdev-home" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1710,8 +1710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2071,23 +2071,23 @@
         <v>1242</v>
       </c>
       <c r="L6" s="5">
-        <v>1125</v>
+        <v>1366</v>
       </c>
       <c r="M6" s="3">
         <f t="shared" si="4"/>
-        <v>2.7173913043478262</v>
+        <v>3.2995169082125604</v>
       </c>
       <c r="N6" s="3">
         <f t="shared" si="5"/>
-        <v>0.90579710144927539</v>
+        <v>1.0998389694041868</v>
       </c>
       <c r="O6" t="str">
         <f t="shared" si="6"/>
-        <v>(-)</v>
+        <v>(+)</v>
       </c>
       <c r="P6" s="1">
         <f t="shared" si="7"/>
-        <v>-7.8188405797101432E-3</v>
+        <v>8.286634460547504E-3</v>
       </c>
       <c r="Q6" s="2">
         <v>1600</v>

</xml_diff>

<commit_message>
Removed usage of csv files. Config files are Excel files now.
</commit_message>
<xml_diff>
--- a/data/datafile.xlsx
+++ b/data/datafile.xlsx
@@ -1,56 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FA3F03-FD8F-D546-98A4-3E235DAAA308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="webdev-home" sheetId="1" r:id="rId1"/>
-    <sheet name="webdev-mainline" sheetId="2" r:id="rId2"/>
+    <sheet sheetId="1" name="webdev-home" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="webdev-mainline" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>usage</t>
   </si>
@@ -99,46 +61,29 @@
   <si>
     <t>chosenWaste</t>
   </si>
-  <si>
-    <t>uniques</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF99D07A"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -150,18 +95,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left style="thin"/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color auto="1"/>
-      </left>
+      <left style="double"/>
       <right/>
       <top/>
       <bottom/>
@@ -171,14 +112,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -187,7 +127,17 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFD4EDD2"/>
+          <bgColor rgb="FF99D07A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFC0504D"/>
         </patternFill>
       </fill>
     </dxf>
@@ -202,12 +152,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFC0504D"/>
+          <bgColor rgb="FFD4EDD2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -219,9 +166,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFD4EDD2"/>
+          <bgColor rgb="FFC0504D"/>
         </patternFill>
       </fill>
     </dxf>
@@ -236,12 +186,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFC0504D"/>
+          <bgColor rgb="FFD4EDD2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -253,9 +200,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFD4EDD2"/>
+          <bgColor rgb="FFC0504D"/>
         </patternFill>
       </fill>
     </dxf>
@@ -270,12 +220,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFC0504D"/>
+          <bgColor rgb="FFD4EDD2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -287,9 +234,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFD4EDD2"/>
+          <bgColor rgb="FFC0504D"/>
         </patternFill>
       </fill>
     </dxf>
@@ -304,19 +254,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFC0504D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF99D07A"/>
+          <bgColor rgb="FFD4EDD2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -654,34 +594,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P17"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="5" customWidth="1"/>
+    <col min="6" max="6" width="21" style="2" customWidth="1"/>
+    <col min="7" max="8" width="23" style="3" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="15" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19" style="4" customWidth="1"/>
+    <col min="12" max="12" width="20" style="5" customWidth="1"/>
+    <col min="13" max="14" width="22" style="3" customWidth="1"/>
+    <col min="15" max="15" width="16" customWidth="1"/>
+    <col min="16" max="16" width="15" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,13 +663,10 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0.13900000000000001</v>
+        <v>0.139</v>
       </c>
       <c r="B2">
         <v>375</v>
@@ -755,50 +685,38 @@
       </c>
       <c r="G2" s="3">
         <f t="shared" ref="G2:G17" si="0">F2/D2</f>
-        <v>3.1197411003236244</v>
       </c>
       <c r="H2" s="3">
-        <f t="shared" ref="H2:H17" si="1">G2/MIN(2,C2)</f>
-        <v>1.5598705501618122</v>
-      </c>
-      <c r="I2" t="str">
+        <f t="shared" ref="H2:H17" si="1">G2/MIN(3,C2)</f>
+      </c>
+      <c r="I2">
         <f t="shared" ref="I2:I17" si="2">_xlfn.IFS(    H2&lt;0.9, "POOR (--)",     H2&lt;1, "(-)",     H2=1, "GOOD!",     H2&gt;1.2, "BIG (++)",     H2&gt;1, "(+)"  )</f>
-        <v>BIG (++)</v>
       </c>
       <c r="J2" s="1">
         <f t="shared" ref="J2:J17" si="3">(H2-1)*A2</f>
-        <v>7.7822006472491906E-2</v>
       </c>
       <c r="K2" s="4">
-        <v>618</v>
+        <v>927</v>
       </c>
       <c r="L2" s="5">
-        <v>692</v>
+        <v>1038</v>
       </c>
       <c r="M2" s="3">
         <f t="shared" ref="M2:M17" si="4">L2/D2</f>
-        <v>2.2394822006472492</v>
       </c>
       <c r="N2" s="3">
-        <f t="shared" ref="N2:N17" si="5">M2/MIN(2,C2)</f>
-        <v>1.1197411003236246</v>
-      </c>
-      <c r="O2" t="str">
+        <f t="shared" ref="N2:N17" si="5">M2/MIN(3,C2)</f>
+      </c>
+      <c r="O2">
         <f t="shared" ref="O2:O17" si="6">_xlfn.IFS(    N2&lt;0.9, "POOR (--)",     N2&lt;1, "(-)",     N2=1, "GOOD!",     N2&gt;1.2, "BIG (++)",     N2&gt;1, "(+)"  )</f>
-        <v>(+)</v>
       </c>
       <c r="P2" s="1">
         <f t="shared" ref="P2:P17" si="7">(N2-1)*A2</f>
-        <v>1.6644012944983824E-2</v>
-      </c>
-      <c r="Q2" s="2" cm="1">
-        <f t="array" ref="Q2:Q4">_xlfn._xlws.SORT(_xlfn.UNIQUE(L2:L17))</f>
-        <v>558</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>0.13400000000000001</v>
+        <v>0.134</v>
       </c>
       <c r="B3">
         <v>414</v>
@@ -817,49 +735,38 @@
       </c>
       <c r="G3" s="3">
         <f t="shared" si="0"/>
-        <v>2.1416184971098264</v>
       </c>
       <c r="H3" s="3">
         <f t="shared" si="1"/>
-        <v>1.0708092485549132</v>
-      </c>
-      <c r="I3" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="2"/>
       </c>
       <c r="J3" s="1">
         <f t="shared" si="3"/>
-        <v>9.4884393063583723E-3</v>
       </c>
       <c r="K3" s="4">
         <v>692</v>
       </c>
       <c r="L3" s="5">
-        <v>692</v>
+        <v>1038</v>
       </c>
       <c r="M3" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
       </c>
       <c r="N3" s="3">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="O3" t="str">
-        <f t="shared" si="6"/>
-        <v>GOOD!</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="6"/>
       </c>
       <c r="P3" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>9.5000000000000001E-2</v>
+        <v>0.095</v>
       </c>
       <c r="B4">
         <v>390</v>
@@ -878,49 +785,38 @@
       </c>
       <c r="G4" s="3">
         <f t="shared" si="0"/>
-        <v>2.9845201238390091</v>
       </c>
       <c r="H4" s="3">
         <f t="shared" si="1"/>
-        <v>1.4922600619195046</v>
-      </c>
-      <c r="I4" t="str">
-        <f t="shared" si="2"/>
-        <v>BIG (++)</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>4.676470588235293E-2</v>
       </c>
       <c r="K4" s="4">
-        <v>646</v>
+        <v>969</v>
       </c>
       <c r="L4" s="5">
-        <v>692</v>
+        <v>1038</v>
       </c>
       <c r="M4" s="3">
         <f t="shared" si="4"/>
-        <v>2.1424148606811144</v>
       </c>
       <c r="N4" s="3">
         <f t="shared" si="5"/>
-        <v>1.0712074303405572</v>
-      </c>
-      <c r="O4" t="str">
-        <f t="shared" si="6"/>
-        <v>(+)</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="6"/>
       </c>
       <c r="P4" s="1">
         <f t="shared" si="7"/>
-        <v>6.7647058823529348E-3</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>1116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>8.5999999999999993E-2</v>
+        <v>0.086</v>
       </c>
       <c r="B5">
         <v>375</v>
@@ -939,46 +835,38 @@
       </c>
       <c r="G5" s="3">
         <f t="shared" si="0"/>
-        <v>2.1035598705501619</v>
       </c>
       <c r="H5" s="3">
         <f t="shared" si="1"/>
-        <v>1.051779935275081</v>
-      </c>
-      <c r="I5" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>4.4530744336569623E-3</v>
       </c>
       <c r="K5" s="4">
         <v>618</v>
       </c>
       <c r="L5" s="5">
-        <v>692</v>
+        <v>1038</v>
       </c>
       <c r="M5" s="3">
         <f t="shared" si="4"/>
-        <v>2.2394822006472492</v>
       </c>
       <c r="N5" s="3">
         <f t="shared" si="5"/>
-        <v>1.1197411003236246</v>
-      </c>
-      <c r="O5" t="str">
-        <f t="shared" si="6"/>
-        <v>(+)</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="6"/>
       </c>
       <c r="P5" s="1">
         <f t="shared" si="7"/>
-        <v>1.0297734627831717E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>8.3000000000000004E-2</v>
+        <v>0.083</v>
       </c>
       <c r="B6">
         <v>414</v>
@@ -997,46 +885,38 @@
       </c>
       <c r="G6" s="3">
         <f t="shared" si="0"/>
-        <v>3.1734104046242773</v>
       </c>
       <c r="H6" s="3">
         <f t="shared" si="1"/>
-        <v>1.5867052023121386</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" si="2"/>
-        <v>BIG (++)</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>4.8696531791907506E-2</v>
       </c>
       <c r="K6" s="4">
-        <v>692</v>
+        <v>1038</v>
       </c>
       <c r="L6" s="5">
-        <v>692</v>
+        <v>1038</v>
       </c>
       <c r="M6" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
       </c>
       <c r="N6" s="3">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="O6" t="str">
-        <f t="shared" si="6"/>
-        <v>GOOD!</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="6"/>
       </c>
       <c r="P6" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6.0999999999999999E-2</v>
+        <v>0.061</v>
       </c>
       <c r="B7">
         <v>360</v>
@@ -1055,46 +935,38 @@
       </c>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>3.2677966101694915</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" si="1"/>
-        <v>1.6338983050847458</v>
-      </c>
-      <c r="I7" t="str">
-        <f t="shared" si="2"/>
-        <v>BIG (++)</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>3.8667796610169489E-2</v>
       </c>
       <c r="K7" s="4">
-        <v>590</v>
+        <v>885</v>
       </c>
       <c r="L7" s="5">
-        <v>692</v>
+        <v>1038</v>
       </c>
       <c r="M7" s="3">
         <f t="shared" si="4"/>
-        <v>2.3457627118644067</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="5"/>
-        <v>1.1728813559322033</v>
-      </c>
-      <c r="O7" t="str">
-        <f t="shared" si="6"/>
-        <v>(+)</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="6"/>
       </c>
       <c r="P7" s="1">
         <f t="shared" si="7"/>
-        <v>1.0545762711864403E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>5.2000000000000005E-2</v>
+        <v>0.052</v>
       </c>
       <c r="B8">
         <v>428</v>
@@ -1113,46 +985,38 @@
       </c>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>3.1754874651810585</v>
       </c>
       <c r="H8" s="3">
         <f t="shared" si="1"/>
-        <v>1.5877437325905293</v>
-      </c>
-      <c r="I8" t="str">
-        <f t="shared" si="2"/>
-        <v>BIG (++)</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>3.0562674094707525E-2</v>
       </c>
       <c r="K8" s="4">
-        <v>718</v>
+        <v>1077</v>
       </c>
       <c r="L8" s="5">
-        <v>692</v>
+        <v>1038</v>
       </c>
       <c r="M8" s="3">
         <f t="shared" si="4"/>
-        <v>1.9275766016713092</v>
       </c>
       <c r="N8" s="3">
         <f t="shared" si="5"/>
-        <v>0.96378830083565459</v>
-      </c>
-      <c r="O8" t="str">
-        <f t="shared" si="6"/>
-        <v>(-)</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="6"/>
       </c>
       <c r="P8" s="1">
         <f t="shared" si="7"/>
-        <v>-1.8830083565459616E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>4.0999999999999995E-2</v>
+        <v>0.041</v>
       </c>
       <c r="B9">
         <v>1920</v>
@@ -1171,46 +1035,38 @@
       </c>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>1.0232974910394266</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" si="1"/>
-        <v>1.0232974910394266</v>
-      </c>
-      <c r="I9" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>9.5519713261648948E-4</v>
       </c>
       <c r="K9" s="4">
         <v>558</v>
       </c>
       <c r="L9" s="5">
-        <v>558</v>
+        <v>1038</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="O9" t="str">
-        <f t="shared" si="6"/>
-        <v>GOOD!</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="6"/>
       </c>
       <c r="P9" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>3.7000000000000005E-2</v>
+        <v>0.037</v>
       </c>
       <c r="B10">
         <v>412</v>
@@ -1229,46 +1085,38 @@
       </c>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>2.8023255813953489</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" si="1"/>
-        <v>1.4011627906976745</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="2"/>
-        <v>BIG (++)</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>1.4843023255813957E-2</v>
       </c>
       <c r="K10" s="4">
-        <v>688</v>
+        <v>905</v>
       </c>
       <c r="L10" s="5">
-        <v>692</v>
+        <v>1038</v>
       </c>
       <c r="M10" s="3">
         <f t="shared" si="4"/>
-        <v>2.0116279069767442</v>
       </c>
       <c r="N10" s="3">
         <f t="shared" si="5"/>
-        <v>1.0058139534883721</v>
-      </c>
-      <c r="O10" t="str">
-        <f t="shared" si="6"/>
-        <v>(+)</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="6"/>
       </c>
       <c r="P10" s="1">
         <f t="shared" si="7"/>
-        <v>2.1511627906976784E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>2.3E-2</v>
+        <v>0.023</v>
       </c>
       <c r="B11">
         <v>1440</v>
@@ -1287,46 +1135,38 @@
       </c>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>2.043010752688172</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="1"/>
-        <v>1.021505376344086</v>
-      </c>
-      <c r="I11" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
-        <v>4.94623655913978E-4</v>
       </c>
       <c r="K11" s="4">
         <v>1116</v>
       </c>
       <c r="L11" s="5">
-        <v>1116</v>
+        <v>1038</v>
       </c>
       <c r="M11" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
       </c>
       <c r="N11" s="3">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="O11" t="str">
-        <f t="shared" si="6"/>
-        <v>GOOD!</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="6"/>
       </c>
       <c r="P11" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1.8000000000000002E-2</v>
+        <v>0.018</v>
       </c>
       <c r="B12">
         <v>1366</v>
@@ -1345,46 +1185,38 @@
       </c>
       <c r="G12" s="3">
         <f t="shared" si="0"/>
-        <v>1.0232974910394266</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" si="1"/>
-        <v>1.0232974910394266</v>
-      </c>
-      <c r="I12" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
-        <v>4.1935483870967841E-4</v>
       </c>
       <c r="K12" s="4">
         <v>558</v>
       </c>
-      <c r="L12" s="6">
-        <v>558</v>
+      <c r="L12" s="5">
+        <v>1038</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
       </c>
       <c r="N12" s="3">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="O12" t="str">
-        <f t="shared" si="6"/>
-        <v>GOOD!</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="6"/>
       </c>
       <c r="P12" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1.6E-2</v>
+        <v>0.016</v>
       </c>
       <c r="B13">
         <v>360</v>
@@ -1403,46 +1235,38 @@
       </c>
       <c r="G13" s="3">
         <f t="shared" si="0"/>
-        <v>2.2033898305084745</v>
       </c>
       <c r="H13" s="3">
         <f t="shared" si="1"/>
-        <v>1.1016949152542372</v>
-      </c>
-      <c r="I13" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="3"/>
-        <v>1.6271186440677959E-3</v>
       </c>
       <c r="K13" s="4">
         <v>590</v>
       </c>
       <c r="L13" s="5">
-        <v>692</v>
+        <v>1038</v>
       </c>
       <c r="M13" s="3">
         <f t="shared" si="4"/>
-        <v>2.3457627118644067</v>
       </c>
       <c r="N13" s="3">
         <f t="shared" si="5"/>
-        <v>1.1728813559322033</v>
-      </c>
-      <c r="O13" t="str">
-        <f t="shared" si="6"/>
-        <v>(+)</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="6"/>
       </c>
       <c r="P13" s="1">
         <f t="shared" si="7"/>
-        <v>2.7661016949152534E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="B14">
         <v>768</v>
@@ -1461,46 +1285,38 @@
       </c>
       <c r="G14" s="3">
         <f t="shared" si="0"/>
-        <v>2.043010752688172</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="1"/>
-        <v>1.021505376344086</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="3"/>
-        <v>3.2258064516129E-4</v>
       </c>
       <c r="K14" s="4">
         <v>1116</v>
       </c>
-      <c r="L14" s="6">
-        <v>558</v>
+      <c r="L14" s="5">
+        <v>1038</v>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
       </c>
       <c r="N14" s="3">
         <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="O14" t="str">
-        <f t="shared" si="6"/>
-        <v>POOR (--)</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="6"/>
       </c>
       <c r="P14" s="1">
         <f t="shared" si="7"/>
-        <v>-7.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>1.3999999999999999E-2</v>
+        <v>0.014</v>
       </c>
       <c r="B15">
         <v>393</v>
@@ -1519,46 +1335,38 @@
       </c>
       <c r="G15" s="3">
         <f t="shared" si="0"/>
-        <v>2.9570552147239262</v>
       </c>
       <c r="H15" s="3">
         <f t="shared" si="1"/>
-        <v>1.4785276073619631</v>
-      </c>
-      <c r="I15" t="str">
-        <f t="shared" si="2"/>
-        <v>BIG (++)</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="3"/>
-        <v>6.6993865030674825E-3</v>
       </c>
       <c r="K15" s="4">
-        <v>652</v>
+        <v>897</v>
       </c>
       <c r="L15" s="5">
-        <v>692</v>
+        <v>1038</v>
       </c>
       <c r="M15" s="3">
         <f t="shared" si="4"/>
-        <v>2.1226993865030677</v>
       </c>
       <c r="N15" s="3">
         <f t="shared" si="5"/>
-        <v>1.0613496932515338</v>
-      </c>
-      <c r="O15" t="str">
-        <f t="shared" si="6"/>
-        <v>(+)</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="6"/>
       </c>
       <c r="P15" s="1">
         <f t="shared" si="7"/>
-        <v>8.5889570552147353E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>1.1000000000000001E-2</v>
+        <v>0.011</v>
       </c>
       <c r="B16">
         <v>1536</v>
@@ -1577,46 +1385,38 @@
       </c>
       <c r="G16" s="3">
         <f t="shared" si="0"/>
-        <v>1.3279569892473118</v>
       </c>
       <c r="H16" s="3">
         <f t="shared" si="1"/>
-        <v>1.0623655913978494</v>
-      </c>
-      <c r="I16" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="3"/>
-        <v>6.8602150537634308E-4</v>
       </c>
       <c r="K16" s="4">
         <v>698</v>
       </c>
       <c r="L16" s="5">
-        <v>692</v>
+        <v>1038</v>
       </c>
       <c r="M16" s="3">
         <f t="shared" si="4"/>
-        <v>1.2401433691756272</v>
       </c>
       <c r="N16" s="3">
         <f t="shared" si="5"/>
-        <v>0.99211469534050178</v>
-      </c>
-      <c r="O16" t="str">
-        <f t="shared" si="6"/>
-        <v>(-)</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="6"/>
       </c>
       <c r="P16" s="1">
         <f t="shared" si="7"/>
-        <v>-8.6738351254480385E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="B17">
         <v>320</v>
@@ -1635,106 +1435,91 @@
       </c>
       <c r="G17" s="3">
         <f t="shared" si="0"/>
-        <v>2.2131782945736433</v>
       </c>
       <c r="H17" s="3">
         <f t="shared" si="1"/>
-        <v>1.1065891472868217</v>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="3"/>
-        <v>8.5271317829457339E-4</v>
       </c>
       <c r="K17" s="4">
         <v>516</v>
       </c>
-      <c r="L17" s="6">
-        <v>558</v>
+      <c r="L17" s="5">
+        <v>1038</v>
       </c>
       <c r="M17" s="3">
         <f t="shared" si="4"/>
-        <v>2.1627906976744184</v>
       </c>
       <c r="N17" s="3">
         <f t="shared" si="5"/>
-        <v>1.0813953488372092</v>
-      </c>
-      <c r="O17" t="str">
-        <f t="shared" si="6"/>
-        <v>(+)</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="6"/>
       </c>
       <c r="P17" s="1">
         <f t="shared" si="7"/>
-        <v>6.5116279069767384E-4</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L2:L11 L13 L15:L16">
-    <cfRule type="expression" dxfId="15" priority="1">
+  <conditionalFormatting sqref="L2:L17">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>O2="GOOD!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>O2="POOR (--)"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>O2="BIG (++)"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>OR(O2="(+)",O2="(-)")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F17">
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>I2="GOOD!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>I2="POOR (--)"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>I2="BIG (++)"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>OR(I2="(+)",I2="(-)")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P17"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="5" customWidth="1"/>
+    <col min="6" max="6" width="21" style="2" customWidth="1"/>
+    <col min="7" max="8" width="23" style="3" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="15" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19" style="4" customWidth="1"/>
+    <col min="12" max="12" width="20" style="5" customWidth="1"/>
+    <col min="13" max="14" width="22" style="3" customWidth="1"/>
+    <col min="15" max="15" width="16" customWidth="1"/>
+    <col min="16" max="16" width="15" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1783,13 +1568,10 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0.13900000000000001</v>
+        <v>0.139</v>
       </c>
       <c r="B2">
         <v>375</v>
@@ -1808,50 +1590,38 @@
       </c>
       <c r="G2" s="3">
         <f t="shared" ref="G2:G17" si="0">F2/D2</f>
-        <v>2.9279999999999999</v>
       </c>
       <c r="H2" s="3">
         <f t="shared" ref="H2:H17" si="1">G2/MIN(3,C2)</f>
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="I2" t="str">
+      </c>
+      <c r="I2">
         <f t="shared" ref="I2:I17" si="2">_xlfn.IFS(    H2&lt;0.9, "POOR (--)",     H2&lt;1, "(-)",     H2=1, "GOOD!",     H2&gt;1.2, "BIG (++)",     H2&gt;1, "(+)"  )</f>
-        <v>(-)</v>
       </c>
       <c r="J2" s="1">
         <f t="shared" ref="J2:J17" si="3">(H2-1)*A2</f>
-        <v>-3.3360000000000035E-3</v>
       </c>
       <c r="K2" s="4">
         <v>1125</v>
       </c>
       <c r="L2" s="5">
-        <v>1125</v>
+        <v>1242</v>
       </c>
       <c r="M2" s="3">
         <f t="shared" ref="M2:M17" si="4">L2/D2</f>
-        <v>3</v>
       </c>
       <c r="N2" s="3">
         <f t="shared" ref="N2:N17" si="5">M2/MIN(3,C2)</f>
-        <v>1</v>
-      </c>
-      <c r="O2" t="str">
+      </c>
+      <c r="O2">
         <f t="shared" ref="O2:O17" si="6">_xlfn.IFS(    N2&lt;0.9, "POOR (--)",     N2&lt;1, "(-)",     N2=1, "GOOD!",     N2&gt;1.2, "BIG (++)",     N2&gt;1, "(+)"  )</f>
-        <v>GOOD!</v>
       </c>
       <c r="P2" s="1">
         <f t="shared" ref="P2:P17" si="7">(N2-1)*A2</f>
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2" cm="1">
-        <f t="array" ref="Q2:Q7">_xlfn._xlws.SORT(_xlfn.UNIQUE(L2:L17))</f>
-        <v>750</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>0.13400000000000001</v>
+        <v>0.134</v>
       </c>
       <c r="B3">
         <v>414</v>
@@ -1870,49 +1640,38 @@
       </c>
       <c r="G3" s="3">
         <f t="shared" si="0"/>
-        <v>2.0410628019323673</v>
       </c>
       <c r="H3" s="3">
         <f t="shared" si="1"/>
-        <v>1.0205314009661837</v>
-      </c>
-      <c r="I3" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="2"/>
       </c>
       <c r="J3" s="1">
         <f t="shared" si="3"/>
-        <v>2.7512077294686113E-3</v>
       </c>
       <c r="K3" s="4">
         <v>828</v>
       </c>
       <c r="L3" s="5">
-        <v>828</v>
+        <v>1242</v>
       </c>
       <c r="M3" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
       </c>
       <c r="N3" s="3">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="O3" t="str">
-        <f t="shared" si="6"/>
-        <v>GOOD!</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="6"/>
       </c>
       <c r="P3" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>9.5000000000000001E-2</v>
+        <v>0.095</v>
       </c>
       <c r="B4">
         <v>390</v>
@@ -1931,49 +1690,38 @@
       </c>
       <c r="G4" s="3">
         <f t="shared" si="0"/>
-        <v>2.8153846153846156</v>
       </c>
       <c r="H4" s="3">
         <f t="shared" si="1"/>
-        <v>0.93846153846153857</v>
-      </c>
-      <c r="I4" t="str">
-        <f t="shared" si="2"/>
-        <v>(-)</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>-5.846153846153836E-3</v>
       </c>
       <c r="K4" s="4">
         <v>1170</v>
       </c>
       <c r="L4" s="5">
-        <v>1125</v>
+        <v>1242</v>
       </c>
       <c r="M4" s="3">
         <f t="shared" si="4"/>
-        <v>2.8846153846153846</v>
       </c>
       <c r="N4" s="3">
         <f t="shared" si="5"/>
-        <v>0.96153846153846156</v>
-      </c>
-      <c r="O4" t="str">
-        <f t="shared" si="6"/>
-        <v>(-)</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="6"/>
       </c>
       <c r="P4" s="1">
         <f t="shared" si="7"/>
-        <v>-3.6538461538461516E-3</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>8.5999999999999993E-2</v>
+        <v>0.086</v>
       </c>
       <c r="B5">
         <v>375</v>
@@ -1992,49 +1740,38 @@
       </c>
       <c r="G5" s="3">
         <f t="shared" si="0"/>
-        <v>1.976</v>
       </c>
       <c r="H5" s="3">
         <f t="shared" si="1"/>
-        <v>0.98799999999999999</v>
-      </c>
-      <c r="I5" t="str">
-        <f t="shared" si="2"/>
-        <v>(-)</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>-1.0320000000000008E-3</v>
       </c>
       <c r="K5" s="4">
         <v>750</v>
       </c>
       <c r="L5" s="5">
-        <v>750</v>
+        <v>1242</v>
       </c>
       <c r="M5" s="3">
         <f t="shared" si="4"/>
-        <v>2</v>
       </c>
       <c r="N5" s="3">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="O5" t="str">
-        <f t="shared" si="6"/>
-        <v>GOOD!</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="6"/>
       </c>
       <c r="P5" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>1366</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>8.3000000000000004E-2</v>
+        <v>0.083</v>
       </c>
       <c r="B6">
         <v>414</v>
@@ -2053,49 +1790,38 @@
       </c>
       <c r="G6" s="3">
         <f t="shared" si="0"/>
-        <v>3.0241545893719808</v>
       </c>
       <c r="H6" s="3">
         <f t="shared" si="1"/>
-        <v>1.0080515297906603</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>6.6827697262480175E-4</v>
       </c>
       <c r="K6" s="4">
         <v>1242</v>
       </c>
       <c r="L6" s="5">
-        <v>1366</v>
+        <v>1242</v>
       </c>
       <c r="M6" s="3">
         <f t="shared" si="4"/>
-        <v>3.2995169082125604</v>
       </c>
       <c r="N6" s="3">
         <f t="shared" si="5"/>
-        <v>1.0998389694041868</v>
-      </c>
-      <c r="O6" t="str">
-        <f t="shared" si="6"/>
-        <v>(+)</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="6"/>
       </c>
       <c r="P6" s="1">
         <f t="shared" si="7"/>
-        <v>8.286634460547504E-3</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6.0999999999999999E-2</v>
+        <v>0.061</v>
       </c>
       <c r="B7">
         <v>360</v>
@@ -2114,49 +1840,38 @@
       </c>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>3.05</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" si="1"/>
-        <v>1.0166666666666666</v>
-      </c>
-      <c r="I7" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>1.0166666666666631E-3</v>
       </c>
       <c r="K7" s="4">
         <v>1080</v>
       </c>
       <c r="L7" s="5">
-        <v>1125</v>
+        <v>1242</v>
       </c>
       <c r="M7" s="3">
         <f t="shared" si="4"/>
-        <v>3.125</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="5"/>
-        <v>1.0416666666666667</v>
-      </c>
-      <c r="O7" t="str">
-        <f t="shared" si="6"/>
-        <v>(+)</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="6"/>
       </c>
       <c r="P7" s="1">
         <f t="shared" si="7"/>
-        <v>2.5416666666666712E-3</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>1920</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>5.2000000000000005E-2</v>
+        <v>0.052</v>
       </c>
       <c r="B8">
         <v>428</v>
@@ -2175,46 +1890,38 @@
       </c>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>2.9252336448598131</v>
       </c>
       <c r="H8" s="3">
         <f t="shared" si="1"/>
-        <v>0.97507788161993769</v>
-      </c>
-      <c r="I8" t="str">
-        <f t="shared" si="2"/>
-        <v>(-)</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>-1.2959501557632401E-3</v>
       </c>
       <c r="K8" s="4">
         <v>1284</v>
       </c>
       <c r="L8" s="5">
-        <v>1366</v>
+        <v>1242</v>
       </c>
       <c r="M8" s="3">
         <f t="shared" si="4"/>
-        <v>3.1915887850467288</v>
       </c>
       <c r="N8" s="3">
         <f t="shared" si="5"/>
-        <v>1.0638629283489096</v>
-      </c>
-      <c r="O8" t="str">
-        <f t="shared" si="6"/>
-        <v>(+)</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="6"/>
       </c>
       <c r="P8" s="1">
         <f t="shared" si="7"/>
-        <v>3.3208722741433E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>4.0999999999999995E-2</v>
+        <v>0.041</v>
       </c>
       <c r="B9">
         <v>1920</v>
@@ -2233,46 +1940,38 @@
       </c>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I9" t="str">
-        <f t="shared" si="2"/>
-        <v>GOOD!</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
       </c>
       <c r="K9" s="4">
         <v>1600</v>
       </c>
       <c r="L9" s="5">
-        <v>1600</v>
+        <v>1242</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="O9" t="str">
-        <f t="shared" si="6"/>
-        <v>GOOD!</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="6"/>
       </c>
       <c r="P9" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>3.7000000000000005E-2</v>
+        <v>0.037</v>
       </c>
       <c r="B10">
         <v>412</v>
@@ -2291,46 +1990,38 @@
       </c>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>2.6650485436893203</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" si="1"/>
-        <v>1.0133264424674222</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>4.9307837129462166E-4</v>
       </c>
       <c r="K10" s="4">
         <v>1084</v>
       </c>
       <c r="L10" s="5">
-        <v>1125</v>
+        <v>1242</v>
       </c>
       <c r="M10" s="3">
         <f t="shared" si="4"/>
-        <v>2.7305825242718447</v>
       </c>
       <c r="N10" s="3">
         <f t="shared" si="5"/>
-        <v>1.0382443058067852</v>
-      </c>
-      <c r="O10" t="str">
-        <f t="shared" si="6"/>
-        <v>(+)</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="6"/>
       </c>
       <c r="P10" s="1">
         <f t="shared" si="7"/>
-        <v>1.4150393148510516E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>2.3E-2</v>
+        <v>0.023</v>
       </c>
       <c r="B11">
         <v>1440</v>
@@ -2349,46 +2040,38 @@
       </c>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>1.1111111111111112</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="1"/>
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="I11" t="str">
-        <f t="shared" si="2"/>
-        <v>POOR (--)</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
-        <v>-1.0222222222222221E-2</v>
       </c>
       <c r="K11" s="4">
         <v>2880</v>
       </c>
       <c r="L11" s="5">
-        <v>1920</v>
+        <v>1242</v>
       </c>
       <c r="M11" s="3">
         <f t="shared" si="4"/>
-        <v>1.3333333333333333</v>
       </c>
       <c r="N11" s="3">
         <f t="shared" si="5"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="O11" t="str">
-        <f t="shared" si="6"/>
-        <v>POOR (--)</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="6"/>
       </c>
       <c r="P11" s="1">
         <f t="shared" si="7"/>
-        <v>-7.6666666666666671E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1.8000000000000002E-2</v>
+        <v>0.018</v>
       </c>
       <c r="B12">
         <v>1366</v>
@@ -2407,46 +2090,38 @@
       </c>
       <c r="G12" s="3">
         <f t="shared" si="0"/>
-        <v>1.0453879941434847</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" si="1"/>
-        <v>1.0453879941434847</v>
-      </c>
-      <c r="I12" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
-        <v>8.1698389458272492E-4</v>
       </c>
       <c r="K12" s="4">
         <v>1366</v>
       </c>
       <c r="L12" s="5">
-        <v>1366</v>
+        <v>1242</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
       </c>
       <c r="N12" s="3">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="O12" t="str">
-        <f t="shared" si="6"/>
-        <v>GOOD!</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="6"/>
       </c>
       <c r="P12" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1.6E-2</v>
+        <v>0.016</v>
       </c>
       <c r="B13">
         <v>360</v>
@@ -2465,46 +2140,38 @@
       </c>
       <c r="G13" s="3">
         <f t="shared" si="0"/>
-        <v>2.0583333333333331</v>
       </c>
       <c r="H13" s="3">
         <f t="shared" si="1"/>
-        <v>1.0291666666666666</v>
-      </c>
-      <c r="I13" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="3"/>
-        <v>4.6666666666666504E-4</v>
       </c>
       <c r="K13" s="4">
         <v>720</v>
       </c>
       <c r="L13" s="5">
-        <v>750</v>
+        <v>1242</v>
       </c>
       <c r="M13" s="3">
         <f t="shared" si="4"/>
-        <v>2.0833333333333335</v>
       </c>
       <c r="N13" s="3">
         <f t="shared" si="5"/>
-        <v>1.0416666666666667</v>
-      </c>
-      <c r="O13" t="str">
-        <f t="shared" si="6"/>
-        <v>(+)</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="6"/>
       </c>
       <c r="P13" s="1">
         <f t="shared" si="7"/>
-        <v>6.6666666666666784E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="B14">
         <v>768</v>
@@ -2523,46 +2190,38 @@
       </c>
       <c r="G14" s="3">
         <f t="shared" si="0"/>
-        <v>2.0833333333333335</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="1"/>
-        <v>1.0416666666666667</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="3"/>
-        <v>6.250000000000011E-4</v>
       </c>
       <c r="K14" s="4">
         <v>1536</v>
       </c>
       <c r="L14" s="5">
-        <v>1600</v>
+        <v>1242</v>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="4"/>
-        <v>2.0833333333333335</v>
       </c>
       <c r="N14" s="3">
         <f t="shared" si="5"/>
-        <v>1.0416666666666667</v>
-      </c>
-      <c r="O14" t="str">
-        <f t="shared" si="6"/>
-        <v>(+)</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="6"/>
       </c>
       <c r="P14" s="1">
         <f t="shared" si="7"/>
-        <v>6.250000000000011E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>1.3999999999999999E-2</v>
+        <v>0.014</v>
       </c>
       <c r="B15">
         <v>393</v>
@@ -2581,46 +2240,38 @@
       </c>
       <c r="G15" s="3">
         <f t="shared" si="0"/>
-        <v>2.7938931297709924</v>
       </c>
       <c r="H15" s="3">
         <f t="shared" si="1"/>
-        <v>1.0159611380985427</v>
-      </c>
-      <c r="I15" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="3"/>
-        <v>2.2345593337959798E-4</v>
       </c>
       <c r="K15" s="4">
         <v>1081</v>
       </c>
       <c r="L15" s="5">
-        <v>1125</v>
+        <v>1242</v>
       </c>
       <c r="M15" s="3">
         <f t="shared" si="4"/>
-        <v>2.8625954198473282</v>
       </c>
       <c r="N15" s="3">
         <f t="shared" si="5"/>
-        <v>1.0409437890353921</v>
-      </c>
-      <c r="O15" t="str">
-        <f t="shared" si="6"/>
-        <v>(+)</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="6"/>
       </c>
       <c r="P15" s="1">
         <f t="shared" si="7"/>
-        <v>5.7321304649548914E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>1.1000000000000001E-2</v>
+        <v>0.011</v>
       </c>
       <c r="B16">
         <v>1536</v>
@@ -2639,46 +2290,38 @@
       </c>
       <c r="G16" s="3">
         <f t="shared" si="0"/>
-        <v>1.0416666666666667</v>
       </c>
       <c r="H16" s="3">
         <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="I16" t="str">
-        <f t="shared" si="2"/>
-        <v>POOR (--)</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="3"/>
-        <v>-1.8333333333333331E-3</v>
       </c>
       <c r="K16" s="4">
         <v>1920</v>
       </c>
       <c r="L16" s="5">
-        <v>1920</v>
+        <v>1242</v>
       </c>
       <c r="M16" s="3">
         <f t="shared" si="4"/>
-        <v>1.25</v>
       </c>
       <c r="N16" s="3">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="O16" t="str">
-        <f t="shared" si="6"/>
-        <v>GOOD!</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="6"/>
       </c>
       <c r="P16" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="B17">
         <v>320</v>
@@ -2697,73 +2340,65 @@
       </c>
       <c r="G17" s="3">
         <f t="shared" si="0"/>
-        <v>2.03125</v>
       </c>
       <c r="H17" s="3">
         <f t="shared" si="1"/>
-        <v>1.015625</v>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="2"/>
-        <v>(+)</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="3"/>
-        <v>1.25E-4</v>
       </c>
       <c r="K17" s="4">
         <v>640</v>
       </c>
       <c r="L17" s="5">
-        <v>750</v>
+        <v>1242</v>
       </c>
       <c r="M17" s="3">
         <f t="shared" si="4"/>
-        <v>2.34375</v>
       </c>
       <c r="N17" s="3">
         <f t="shared" si="5"/>
-        <v>1.171875</v>
-      </c>
-      <c r="O17" t="str">
-        <f t="shared" si="6"/>
-        <v>(+)</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="6"/>
       </c>
       <c r="P17" s="1">
         <f t="shared" si="7"/>
-        <v>1.3749999999999999E-3</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L17">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>O2="GOOD!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>O2="POOR (--)"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>O2="BIG (++)"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="11" priority="4">
       <formula>OR(O2="(+)",O2="(-)")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F17">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="12" priority="5">
       <formula>I2="GOOD!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="13" priority="6">
       <formula>I2="POOR (--)"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="14" priority="7">
       <formula>I2="BIG (++)"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="15" priority="8">
       <formula>OR(I2="(+)",I2="(-)")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>